<commit_message>
Use bika IDs for DuplicateAnalysis and Client
</commit_message>
<xml_diff>
--- a/test_setup_data.xlsx
+++ b/test_setup_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="7" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="894" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="23" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="726" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="1" state="visible" r:id="rId2"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4854" uniqueCount="1227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4858" uniqueCount="1230">
   <si>
     <t>Password lifetime</t>
   </si>
@@ -3688,37 +3688,46 @@
     <t>Padding</t>
   </si>
   <si>
+    <t>ARImport</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>client</t>
+  </si>
+  <si>
+    <t>DuplicateAnalysis</t>
+  </si>
+  <si>
+    <t>DA</t>
+  </si>
+  <si>
+    <t>Invoice</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>ReferenceAnalysis</t>
+  </si>
+  <si>
+    <t>RA</t>
+  </si>
+  <si>
+    <t>ReferenceSample</t>
+  </si>
+  <si>
+    <t>RS</t>
+  </si>
+  <si>
+    <t>SupplyOrder</t>
+  </si>
+  <si>
     <t>Worksheet</t>
   </si>
   <si>
     <t>WS</t>
-  </si>
-  <si>
-    <t>SupplyOrder</t>
-  </si>
-  <si>
-    <t>Invoice</t>
-  </si>
-  <si>
-    <t>I</t>
-  </si>
-  <si>
-    <t>ARImport</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>ReferenceSample</t>
-  </si>
-  <si>
-    <t>RS</t>
-  </si>
-  <si>
-    <t>ReferenceAnalysis</t>
-  </si>
-  <si>
-    <t>RA</t>
   </si>
 </sst>
 </file>
@@ -4087,11 +4096,11 @@
   <dimension ref="A2:N4"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="F7" activeCellId="0" pane="topLeft" sqref="F7"/>
+      <selection activeCell="F7" activeCellId="1" pane="topLeft" sqref="A5:IV5 F7"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="257" min="1" style="1" width="13.6588235294118"/>
+    <col collapsed="false" hidden="false" max="257" min="1" style="1" width="13.7294117647059"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2" s="2"/>
@@ -4199,14 +4208,14 @@
   <dimension ref="A1:M47"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C1" activeCellId="0" pane="topLeft" sqref="C1"/>
+      <selection activeCell="C1" activeCellId="1" pane="topLeft" sqref="A5:IV5 C1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="21" width="32.4980392156863"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="42.8509803921569"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="7" width="17.4392156862745"/>
-    <col collapsed="false" hidden="false" max="257" min="5" style="7" width="14.0823529411765"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="21" width="32.6588235294118"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="43.0705882352941"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="7" width="17.5294117647059"/>
+    <col collapsed="false" hidden="false" max="257" min="5" style="7" width="14.1529411764706"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1" s="8">
@@ -5027,14 +5036,14 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="A5:IV5 A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="30" width="23.5529411764706"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="30" width="52.1411764705882"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="30" width="28.1098039215686"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="30" width="14.0823529411765"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="30" width="23.6705882352941"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="30" width="52.4039215686275"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="30" width="28.2549019607843"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="30" width="14.1529411764706"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="1" s="31">
@@ -5181,14 +5190,14 @@
   <dimension ref="A1:V14"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A7" activeCellId="0" pane="topLeft" sqref="A7"/>
+      <selection activeCell="A7" activeCellId="1" pane="topLeft" sqref="A5:IV5 A7"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="30.6235294117647"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="7" width="79.3098039215686"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="7" width="27.9450980392157"/>
-    <col collapsed="false" hidden="false" max="257" min="5" style="7" width="14.0823529411765"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="30.7764705882353"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="7" width="79.7058823529412"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="7" width="28.0823529411765"/>
+    <col collapsed="false" hidden="false" max="257" min="5" style="7" width="14.1529411764706"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1" s="8">
@@ -5414,37 +5423,37 @@
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <pane activePane="bottomLeft" topLeftCell="A251" xSplit="0" ySplit="1170"/>
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
-      <selection activeCell="Q263" activeCellId="0" pane="bottomLeft" sqref="Q263"/>
+      <selection activeCell="Q263" activeCellId="1" pane="bottomLeft" sqref="A5:IV5 Q263"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="20" width="14.5176470588235"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="20" width="21.5803921568627"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="20" width="10.8627450980392"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="20" width="10.3647058823529"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="20" width="14.1529411764706"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="33" width="8.92549019607843"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="20" width="14.8588235294118"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="20" width="9.10588235294118"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="20" width="7.15294117647059"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="20" width="7.29803921568627"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="20" width="8.57254901960784"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="20" width="7.04705882352941"/>
-    <col collapsed="false" hidden="false" max="15" min="14" style="20" width="7.29803921568627"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="20" width="5.87058823529412"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="20" width="9.47843137254902"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="20" width="9.10588235294118"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="20" width="15.0235294117647"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="20" width="11.5960784313726"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="33" width="9.29019607843137"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="20" width="17.1490196078431"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="17" width="12.9529411764706"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="20" width="14.0823529411765"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="7" width="8.25882352941177"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="7" width="39.2901960784314"/>
-    <col collapsed="false" hidden="false" max="28" min="27" style="7" width="14.0823529411765"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="27" width="12.9529411764706"/>
-    <col collapsed="false" hidden="false" max="257" min="30" style="27" width="14.0823529411765"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="20" width="14.5882352941176"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="20" width="21.6901960784314"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="20" width="10.9176470588235"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="20" width="10.4117647058824"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="20" width="14.2274509803922"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="33" width="8.97254901960784"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="20" width="14.9333333333333"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="20" width="9.15294117647059"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="20" width="7.1921568627451"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="20" width="7.33333333333333"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="20" width="8.61176470588235"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="20" width="7.08235294117647"/>
+    <col collapsed="false" hidden="false" max="15" min="14" style="20" width="7.33333333333333"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="20" width="5.90588235294118"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="20" width="9.52549019607843"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="20" width="9.15294117647059"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="20" width="15.1058823529412"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="20" width="11.6588235294118"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="33" width="9.33333333333333"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="20" width="17.2313725490196"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="17" width="13.0156862745098"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="20" width="14.1529411764706"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="7" width="8.30196078431373"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="7" width="39.4862745098039"/>
+    <col collapsed="false" hidden="false" max="28" min="27" style="7" width="14.1529411764706"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="27" width="13.0156862745098"/>
+    <col collapsed="false" hidden="false" max="257" min="30" style="27" width="14.1529411764706"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="24.25" outlineLevel="0" r="1" s="22">
@@ -6505,7 +6514,7 @@
         <v>880</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="23.85" outlineLevel="0" r="39">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="39">
       <c r="A39" s="20" t="s">
         <v>899</v>
       </c>
@@ -9919,7 +9928,7 @@
         <v>880</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="23.85" outlineLevel="0" r="180">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="180">
       <c r="A180" s="20" t="s">
         <v>961</v>
       </c>
@@ -12150,15 +12159,15 @@
   <dimension ref="A1:E2159"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A6" activeCellId="0" pane="topLeft" sqref="A6"/>
+      <selection activeCell="A6" activeCellId="1" pane="topLeft" sqref="A5:IV5 A6"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="20" width="26.8156862745098"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="20" width="21.5803921568627"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="20" width="14.443137254902"/>
-    <col collapsed="false" hidden="false" max="227" min="4" style="27" width="14.0823529411765"/>
-    <col collapsed="false" hidden="false" max="257" min="228" style="0" width="9.92156862745098"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="20" width="26.9529411764706"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="20" width="21.6901960784314"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="20" width="14.5176470588235"/>
+    <col collapsed="false" hidden="false" max="227" min="4" style="27" width="14.1529411764706"/>
+    <col collapsed="false" hidden="false" max="257" min="228" style="0" width="9.97647058823529"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="24.25" outlineLevel="0" r="1" s="22">
@@ -43485,20 +43494,20 @@
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="B15" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D29" activeCellId="0" pane="topLeft" sqref="D29"/>
+      <selection activeCell="D29" activeCellId="1" pane="topLeft" sqref="A5:IV5 D29"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="21.9058823529412"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="23.2"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="16.0823529411765"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="7" width="49.2470588235294"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="7" width="21.1294117647059"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="7" width="16.9411764705882"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="7" width="7.29803921568627"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="7" width="8.57254901960784"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="7" width="6.31372549019608"/>
-    <col collapsed="false" hidden="false" max="257" min="10" style="7" width="14.0823529411765"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="22.0156862745098"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="23.3176470588235"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="16.1607843137255"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="7" width="49.4901960784314"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="7" width="21.2352941176471"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="7" width="17.0196078431373"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="7" width="7.33333333333333"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="7" width="8.61176470588235"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="7" width="6.34117647058824"/>
+    <col collapsed="false" hidden="false" max="257" min="10" style="7" width="14.1529411764706"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="16.55" outlineLevel="0" r="1" s="8">
@@ -44194,15 +44203,15 @@
   <dimension ref="A1:V7"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D6" activeCellId="0" pane="topLeft" sqref="D6"/>
+      <selection activeCell="D6" activeCellId="1" pane="topLeft" sqref="A5:IV5 D6"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.2117647058823"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.8627450980392"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.81960784313726"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.7843137254902"/>
-    <col collapsed="false" hidden="false" max="257" min="5" style="0" width="8.81960784313726"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.3372549019608"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.0549019607843"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.86274509803922"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.9725490196078"/>
+    <col collapsed="false" hidden="false" max="257" min="5" style="0" width="8.86274509803922"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1" s="39">
@@ -44334,14 +44343,14 @@
   <dimension ref="A1:V5"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="A5:IV5 A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="23.2"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="57.4862745098039"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="56.8274509803922"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="7" width="14.0823529411765"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="23.3176470588235"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="57.7764705882353"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="57.1058823529412"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="7" width="14.1529411764706"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1" s="10">
@@ -44421,17 +44430,17 @@
   <dimension ref="A1:W79"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B11" activeCellId="0" pane="topLeft" sqref="B11"/>
+      <selection activeCell="B11" activeCellId="1" pane="topLeft" sqref="A5:IV5 B11"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="27" width="24.5725490196078"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="27" width="37.3176470588235"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="27" width="14.0823529411765"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="27" width="13.8745098039216"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="27" width="9.81176470588235"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="27" width="7.94901960784314"/>
-    <col collapsed="false" hidden="false" max="257" min="9" style="27" width="14.0823529411765"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="27" width="24.6901960784314"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="27" width="37.5058823529412"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="27" width="14.1529411764706"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="27" width="13.9372549019608"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="27" width="9.85882352941177"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="27" width="7.9843137254902"/>
+    <col collapsed="false" hidden="false" max="257" min="9" style="27" width="14.1529411764706"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1" s="26">
@@ -45667,18 +45676,18 @@
   <dimension ref="A1:W6"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="A5:IV5 A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="30" width="13.6313725490196"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="30" width="21.5803921568627"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="30" width="23.3176470588235"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="30" width="18.3137254901961"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="30" width="18.1333333333333"/>
-    <col collapsed="false" hidden="false" max="8" min="6" style="30" width="14.0823529411765"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="30" width="33.8352941176471"/>
-    <col collapsed="false" hidden="false" max="257" min="11" style="30" width="14.0823529411765"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="30" width="13.7019607843137"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="30" width="21.6901960784314"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="30" width="23.4352941176471"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="30" width="18.4039215686275"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="30" width="18.2235294117647"/>
+    <col collapsed="false" hidden="false" max="8" min="6" style="30" width="14.1529411764706"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="30" width="34.0078431372549"/>
+    <col collapsed="false" hidden="false" max="257" min="11" style="30" width="14.1529411764706"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="1" s="31">
@@ -45827,17 +45836,17 @@
   <dimension ref="A2:M4"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="H4" activeCellId="0" pane="topLeft" sqref="H4"/>
+      <selection activeCell="H4" activeCellId="1" pane="topLeft" sqref="A5:IV5 H4"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="9.52549019607843"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="12.4196078431373"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="5" width="13.6588235294118"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="23.3176470588235"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="5" width="23.8588235294118"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="12.0823529411765"/>
-    <col collapsed="false" hidden="false" max="257" min="8" style="5" width="13.6588235294118"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="9.56862745098039"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="12.4823529411765"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="5" width="13.7294117647059"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="23.4352941176471"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="5" width="23.9764705882353"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="12.1372549019608"/>
+    <col collapsed="false" hidden="false" max="257" min="8" style="5" width="13.7294117647059"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2" s="2"/>
@@ -45948,19 +45957,19 @@
   <dimension ref="A1:W6"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="A5:IV5 A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="30" width="25.9019607843137"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="30" width="21.5803921568627"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="30" width="23.3176470588235"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="30" width="18.3137254901961"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="30" width="18.1333333333333"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="30" width="29.8901960784314"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="30" width="14.0823529411765"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="30" width="33.8352941176471"/>
-    <col collapsed="false" hidden="false" max="257" min="11" style="30" width="14.0823529411765"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="30" width="26.0313725490196"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="30" width="21.6901960784314"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="30" width="23.4352941176471"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="30" width="18.4039215686275"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="30" width="18.2235294117647"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="30" width="30.0352941176471"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="30" width="14.1529411764706"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="30" width="34.0078431372549"/>
+    <col collapsed="false" hidden="false" max="257" min="11" style="30" width="14.1529411764706"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="1" s="31">
@@ -46106,13 +46115,13 @@
   <dimension ref="A1:V7"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="A5:IV5 A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="23.2"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="41.8117647058824"/>
-    <col collapsed="false" hidden="false" max="257" min="3" style="7" width="14.0823529411765"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="23.3176470588235"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="42.0196078431373"/>
+    <col collapsed="false" hidden="false" max="257" min="3" style="7" width="14.1529411764706"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1" s="10">
@@ -46208,15 +46217,15 @@
   <dimension ref="A1:V23"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="A5:IV5 A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="46.9960784313725"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="28.8352941176471"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="7" width="14.0823529411765"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="7" width="18.3137254901961"/>
-    <col collapsed="false" hidden="false" max="257" min="6" style="7" width="14.0823529411765"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="47.2313725490196"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="28.9764705882353"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="7" width="14.1529411764706"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="7" width="18.4039215686275"/>
+    <col collapsed="false" hidden="false" max="257" min="6" style="7" width="14.1529411764706"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1" s="10">
@@ -46613,20 +46622,20 @@
   <dimension ref="A1:V43"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="G3" activeCellId="0" pane="topLeft" sqref="G3"/>
+      <selection activeCell="G3" activeCellId="1" pane="topLeft" sqref="A5:IV5 G3"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="27" width="23.0352941176471"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="27" width="23.3176470588235"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="27" width="29.1764705882353"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="27" width="11.7137254901961"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="27" width="8.10196078431373"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="27" width="25.243137254902"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="27" width="16.6039215686275"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="25.243137254902"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="16.6039215686275"/>
-    <col collapsed="false" hidden="false" max="257" min="12" style="27" width="14.0823529411765"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="27" width="23.1529411764706"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="27" width="23.4352941176471"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="27" width="29.321568627451"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="27" width="11.7764705882353"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="27" width="8.14117647058824"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="27" width="25.3686274509804"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="27" width="16.6862745098039"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="25.3686274509804"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="16.6862745098039"/>
+    <col collapsed="false" hidden="false" max="257" min="12" style="27" width="14.1529411764706"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1" s="26">
@@ -47112,16 +47121,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:V9"/>
+  <dimension ref="A1:V11"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B2" activeCellId="0" pane="topLeft" sqref="B2"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="C5" activeCellId="0" pane="topLeft" sqref="A5:IV5"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="23.2"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="15.3764705882353"/>
-    <col collapsed="false" hidden="false" max="257" min="3" style="7" width="14.0823529411765"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="23.3176470588235"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="15.4549019607843"/>
+    <col collapsed="false" hidden="false" max="257" min="3" style="7" width="14.1529411764706"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1" s="10">
@@ -47185,14 +47194,12 @@
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="5">
       <c r="A5" s="27" t="s">
+        <v>331</v>
+      </c>
+      <c r="B5" s="27" t="s">
         <v>1218</v>
       </c>
-      <c r="B5" s="27" t="s">
-        <v>773</v>
-      </c>
-      <c r="C5" s="27" t="n">
-        <v>3</v>
-      </c>
+      <c r="C5" s="27"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="6">
       <c r="A6" s="27" t="s">
@@ -47202,7 +47209,7 @@
         <v>1220</v>
       </c>
       <c r="C6" s="27" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="7">
@@ -47213,7 +47220,7 @@
         <v>1222</v>
       </c>
       <c r="C7" s="27" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="8">
@@ -47236,6 +47243,28 @@
       </c>
       <c r="C9" s="27" t="n">
         <v>4</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="10">
+      <c r="A10" s="27" t="s">
+        <v>1227</v>
+      </c>
+      <c r="B10" s="27" t="s">
+        <v>773</v>
+      </c>
+      <c r="C10" s="27" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="11">
+      <c r="A11" s="27" t="s">
+        <v>1228</v>
+      </c>
+      <c r="B11" s="27" t="s">
+        <v>1229</v>
+      </c>
+      <c r="C11" s="27" t="n">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -47257,18 +47286,18 @@
   <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="F33" activeCellId="0" pane="topLeft" sqref="F33"/>
+      <selection activeCell="F33" activeCellId="1" pane="topLeft" sqref="A5:IV5 F33"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="13.4666666666667"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="14.1529411764706"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="20.7764705882353"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="7" width="16.443137254902"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="7" width="16.0823529411765"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="7" width="36.0588235294118"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="7" width="22.6117647058824"/>
-    <col collapsed="false" hidden="false" max="257" min="8" style="7" width="14.0823529411765"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="13.5294117647059"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="14.2274509803922"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="20.8823529411765"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="7" width="16.5254901960784"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="7" width="16.1607843137255"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="7" width="36.2392156862745"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="7" width="22.7294117647059"/>
+    <col collapsed="false" hidden="false" max="257" min="8" style="7" width="14.1529411764706"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1" s="9">
@@ -48238,22 +48267,22 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="J5" activeCellId="0" pane="topLeft" sqref="J5"/>
+      <selection activeCell="J5" activeCellId="0" pane="topLeft" sqref="A5:IV5"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="17.1843137254902"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="13.7764705882353"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="12.5098039215686"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="7" width="26.9882352941176"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="7" width="20.1607843137255"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="7" width="16.9843137254902"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="7" width="19.6627450980392"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="7" width="17.1843137254902"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="7" width="21.8862745098039"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="7" width="16.5686274509804"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="7" width="50.3607843137255"/>
-    <col collapsed="false" hidden="false" max="257" min="12" style="7" width="14.0823529411765"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="17.2666666666667"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="13.8470588235294"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="12.5725490196078"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="7" width="27.1254901960784"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="7" width="20.2666666666667"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="7" width="17.0666666666667"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="7" width="19.7607843137255"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="7" width="17.2666666666667"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="7" width="21.9960784313725"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="7" width="16.6509803921569"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="7" width="50.6117647058824"/>
+    <col collapsed="false" hidden="false" max="257" min="12" style="7" width="14.1529411764706"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1" s="10">
@@ -48595,14 +48624,14 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="F16" activeCellId="0" pane="topLeft" sqref="F16"/>
+      <selection activeCell="F16" activeCellId="1" pane="topLeft" sqref="A5:IV5 F16"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="21.5803921568627"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="39.2352941176471"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="29.121568627451"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="7" width="14.0823529411765"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="21.6901960784314"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="39.4313725490196"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="29.2666666666667"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="7" width="14.1529411764706"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1" s="8">
@@ -48687,17 +48716,17 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="A5:IV5 A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="11" width="17.6823529411765"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="12" width="23.8588235294118"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="12" width="16.0823529411765"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="12" width="26.5803921568627"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="12" width="16.243137254902"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="12" width="17.4392156862745"/>
-    <col collapsed="false" hidden="false" max="257" min="7" style="12" width="14.0823529411765"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="11" width="17.7725490196078"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="12" width="23.9764705882353"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="12" width="16.1607843137255"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="12" width="26.7176470588235"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="12" width="16.3254901960784"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="12" width="17.5294117647059"/>
+    <col collapsed="false" hidden="false" max="257" min="7" style="12" width="14.1529411764706"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="11.6" outlineLevel="0" r="1" s="15">
@@ -48958,27 +48987,27 @@
   <dimension ref="A1:P21"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C11" activeCellId="0" pane="topLeft" sqref="C11"/>
+      <selection activeCell="C11" activeCellId="1" pane="topLeft" sqref="A5:IV5 C11"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="12" width="23.8588235294118"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="12" width="14.0823529411765"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="12" width="11.3764705882353"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="12" width="18.3137254901961"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="12" width="23.2"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="12" width="20.0235294117647"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="12" width="15.5294117647059"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="12" width="16.0823529411765"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="12" width="15.7294117647059"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="12" width="16.6039215686275"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="12" width="13.1411764705882"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="12" width="20.0235294117647"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="12" width="30.0549019607843"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="12" width="14.1529411764706"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="12" width="14.0823529411765"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="16" width="19.8627450980392"/>
-    <col collapsed="false" hidden="false" max="257" min="17" style="12" width="14.0823529411765"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="12" width="23.9764705882353"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="12" width="14.1529411764706"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="12" width="11.4313725490196"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="12" width="18.4039215686275"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="12" width="23.3176470588235"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="12" width="20.1254901960784"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="12" width="15.6117647058824"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="12" width="16.1607843137255"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="12" width="15.8078431372549"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="12" width="16.6862745098039"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="12" width="13.2039215686275"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="12" width="20.1254901960784"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="12" width="30.2078431372549"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="12" width="14.2274509803922"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="12" width="14.1529411764706"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="16" width="19.9607843137255"/>
+    <col collapsed="false" hidden="false" max="257" min="17" style="12" width="14.1529411764706"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="11.6" outlineLevel="0" r="1" s="15">
@@ -50039,20 +50068,20 @@
   </sheetPr>
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="D1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="I24" activeCellId="0" pane="topLeft" sqref="I24"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="D1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="G26" activeCellId="1" pane="topLeft" sqref="A5:IV5 G26"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="17" width="29.1764705882353"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="17" width="41.9921568627451"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="17" width="47.1490196078431"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="17" width="19.5254901960784"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="17" width="33.3294117647059"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="17" width="14.0823529411765"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="17" width="26.2666666666667"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="17" width="23.9058823529412"/>
-    <col collapsed="false" hidden="false" max="257" min="9" style="17" width="14.0823529411765"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="17" width="29.321568627451"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="17" width="42.2"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="17" width="47.3843137254902"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="17" width="19.6274509803922"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="17" width="33.5019607843137"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="17" width="14.1529411764706"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="17" width="26.4"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="17" width="24.0313725490196"/>
+    <col collapsed="false" hidden="false" max="257" min="9" style="17" width="14.1529411764706"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1" s="19">
@@ -50686,20 +50715,20 @@
   <dimension ref="A1:T14"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="A5:IV5 A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="21" width="19.1725490196078"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="28.4549019607843"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="7.29803921568627"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="7" width="8.41960784313726"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="7" width="10.6980392156863"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="7" width="13.7294117647059"/>
-    <col collapsed="false" hidden="false" max="10" min="7" style="7" width="6.21176470588235"/>
-    <col collapsed="false" hidden="false" max="14" min="11" style="7" width="7.29803921568627"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="7" width="12.9529411764706"/>
-    <col collapsed="false" hidden="false" max="257" min="16" style="7" width="14.0823529411765"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="21" width="19.2745098039216"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="28.6"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="7.33333333333333"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="7" width="8.45490196078431"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="7" width="10.7529411764706"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="7" width="13.8"/>
+    <col collapsed="false" hidden="false" max="10" min="7" style="7" width="6.25098039215686"/>
+    <col collapsed="false" hidden="false" max="14" min="11" style="7" width="7.33333333333333"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="7" width="13.0156862745098"/>
+    <col collapsed="false" hidden="false" max="257" min="16" style="7" width="14.1529411764706"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="13.05" outlineLevel="0" r="1" s="8">

</xml_diff>

<commit_message>
Invalid analysis result may be submitted for verification
closes #17
</commit_message>
<xml_diff>
--- a/test_setup_data.xlsx
+++ b/test_setup_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="23" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="726" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="23" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="589" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="1" state="visible" r:id="rId2"/>
@@ -4096,11 +4096,11 @@
   <dimension ref="A2:N4"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="F7" activeCellId="1" pane="topLeft" sqref="A5:IV5 F7"/>
+      <selection activeCell="F7" activeCellId="0" pane="topLeft" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="257" min="1" style="1" width="13.7294117647059"/>
+    <col collapsed="false" hidden="false" max="257" min="1" style="1" width="13.8"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2" s="2"/>
@@ -4208,14 +4208,14 @@
   <dimension ref="A1:M47"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C1" activeCellId="1" pane="topLeft" sqref="A5:IV5 C1"/>
+      <selection activeCell="C1" activeCellId="0" pane="topLeft" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="21" width="32.6588235294118"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="43.0705882352941"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="7" width="17.5294117647059"/>
-    <col collapsed="false" hidden="false" max="257" min="5" style="7" width="14.1529411764706"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="21" width="32.8235294117647"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="43.2862745098039"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="7" width="17.6196078431373"/>
+    <col collapsed="false" hidden="false" max="257" min="5" style="7" width="14.2274509803922"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1" s="8">
@@ -5036,14 +5036,14 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="A5:IV5 A1"/>
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="30" width="23.6705882352941"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="30" width="52.4039215686275"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="30" width="28.2549019607843"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="30" width="14.1529411764706"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="30" width="23.7882352941176"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="30" width="52.6666666666667"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="30" width="28.4"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="30" width="14.2274509803922"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="1" s="31">
@@ -5190,14 +5190,14 @@
   <dimension ref="A1:V14"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A7" activeCellId="1" pane="topLeft" sqref="A5:IV5 A7"/>
+      <selection activeCell="A7" activeCellId="0" pane="topLeft" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="30.7764705882353"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="7" width="79.7058823529412"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="7" width="28.0823529411765"/>
-    <col collapsed="false" hidden="false" max="257" min="5" style="7" width="14.1529411764706"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="30.9333333333333"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="7" width="80.1058823529412"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="7" width="28.2196078431373"/>
+    <col collapsed="false" hidden="false" max="257" min="5" style="7" width="14.2274509803922"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1" s="8">
@@ -5423,37 +5423,37 @@
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <pane activePane="bottomLeft" topLeftCell="A251" xSplit="0" ySplit="1170"/>
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
-      <selection activeCell="Q263" activeCellId="1" pane="bottomLeft" sqref="A5:IV5 Q263"/>
+      <selection activeCell="Q263" activeCellId="0" pane="bottomLeft" sqref="Q263"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="20" width="14.5882352941176"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="20" width="21.6901960784314"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="20" width="10.9176470588235"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="20" width="10.4117647058824"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="20" width="14.2274509803922"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="33" width="8.97254901960784"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="20" width="14.9333333333333"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="20" width="9.15294117647059"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="20" width="7.1921568627451"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="20" width="7.33333333333333"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="20" width="8.61176470588235"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="20" width="7.08235294117647"/>
-    <col collapsed="false" hidden="false" max="15" min="14" style="20" width="7.33333333333333"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="20" width="5.90588235294118"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="20" width="9.52549019607843"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="20" width="9.15294117647059"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="20" width="15.1058823529412"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="20" width="11.6588235294118"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="33" width="9.33333333333333"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="20" width="17.2313725490196"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="17" width="13.0156862745098"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="20" width="14.1529411764706"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="7" width="8.30196078431373"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="7" width="39.4862745098039"/>
-    <col collapsed="false" hidden="false" max="28" min="27" style="7" width="14.1529411764706"/>
-    <col collapsed="false" hidden="false" max="29" min="29" style="27" width="13.0156862745098"/>
-    <col collapsed="false" hidden="false" max="257" min="30" style="27" width="14.1529411764706"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="20" width="14.6627450980392"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="20" width="21.7960784313725"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="20" width="10.9725490196078"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="20" width="10.4627450980392"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="20" width="14.2980392156863"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="33" width="9.0156862745098"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="20" width="15.0039215686275"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="20" width="9.2"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="20" width="7.22745098039216"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="20" width="7.37254901960784"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="20" width="8.65490196078431"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="20" width="7.11764705882353"/>
+    <col collapsed="false" hidden="false" max="15" min="14" style="20" width="7.37254901960784"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="20" width="5.94117647058824"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="20" width="9.56862745098039"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="20" width="9.2"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="20" width="15.1843137254902"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="20" width="11.7137254901961"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="33" width="9.38039215686275"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="20" width="17.321568627451"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="17" width="13.078431372549"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="20" width="14.2274509803922"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="7" width="8.33725490196079"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="7" width="39.678431372549"/>
+    <col collapsed="false" hidden="false" max="28" min="27" style="7" width="14.2274509803922"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="27" width="13.078431372549"/>
+    <col collapsed="false" hidden="false" max="257" min="30" style="27" width="14.2274509803922"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="24.25" outlineLevel="0" r="1" s="22">
@@ -12159,15 +12159,15 @@
   <dimension ref="A1:E2159"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A6" activeCellId="1" pane="topLeft" sqref="A5:IV5 A6"/>
+      <selection activeCell="A6" activeCellId="0" pane="topLeft" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="20" width="26.9529411764706"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="20" width="21.6901960784314"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="20" width="14.5176470588235"/>
-    <col collapsed="false" hidden="false" max="227" min="4" style="27" width="14.1529411764706"/>
-    <col collapsed="false" hidden="false" max="257" min="228" style="0" width="9.97647058823529"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="20" width="27.0862745098039"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="20" width="21.7960784313725"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="20" width="14.5882352941176"/>
+    <col collapsed="false" hidden="false" max="227" min="4" style="27" width="14.2274509803922"/>
+    <col collapsed="false" hidden="false" max="257" min="228" style="0" width="10.0196078431373"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="24.25" outlineLevel="0" r="1" s="22">
@@ -43494,20 +43494,20 @@
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="B15" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D29" activeCellId="1" pane="topLeft" sqref="A5:IV5 D29"/>
+      <selection activeCell="D29" activeCellId="0" pane="topLeft" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="22.0156862745098"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="23.3176470588235"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="16.1607843137255"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="7" width="49.4901960784314"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="7" width="21.2352941176471"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="7" width="17.0196078431373"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="7" width="7.33333333333333"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="7" width="8.61176470588235"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="7" width="6.34117647058824"/>
-    <col collapsed="false" hidden="false" max="257" min="10" style="7" width="14.1529411764706"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="22.121568627451"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="23.4352941176471"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="16.243137254902"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="7" width="49.7333333333333"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="7" width="21.3450980392157"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="7" width="17.1019607843137"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="7" width="7.37254901960784"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="7" width="8.65490196078431"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="7" width="6.37647058823529"/>
+    <col collapsed="false" hidden="false" max="257" min="10" style="7" width="14.2274509803922"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="16.55" outlineLevel="0" r="1" s="8">
@@ -44203,15 +44203,15 @@
   <dimension ref="A1:V7"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D6" activeCellId="1" pane="topLeft" sqref="A5:IV5 D6"/>
+      <selection activeCell="D6" activeCellId="0" pane="topLeft" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.3372549019608"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.0549019607843"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.86274509803922"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="36.9725490196078"/>
-    <col collapsed="false" hidden="false" max="257" min="5" style="0" width="8.86274509803922"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.4549019607843"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.2509803921569"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="8.90980392156863"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="37.1647058823529"/>
+    <col collapsed="false" hidden="false" max="257" min="5" style="0" width="8.90980392156863"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1" s="39">
@@ -44343,14 +44343,14 @@
   <dimension ref="A1:V5"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="A5:IV5 A1"/>
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="23.3176470588235"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="57.7764705882353"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="57.1058823529412"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="7" width="14.1529411764706"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="23.4352941176471"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="58.0627450980392"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="57.3960784313726"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="7" width="14.2274509803922"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1" s="10">
@@ -44430,17 +44430,17 @@
   <dimension ref="A1:W79"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B11" activeCellId="1" pane="topLeft" sqref="A5:IV5 B11"/>
+      <selection activeCell="B11" activeCellId="0" pane="topLeft" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="27" width="24.6901960784314"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="27" width="37.5058823529412"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="27" width="14.1529411764706"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="27" width="13.9372549019608"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="27" width="9.85882352941177"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="27" width="7.9843137254902"/>
-    <col collapsed="false" hidden="false" max="257" min="9" style="27" width="14.1529411764706"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="27" width="24.8078431372549"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="27" width="37.6862745098039"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="27" width="14.2274509803922"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="27" width="14.0078431372549"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="27" width="9.90196078431373"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="27" width="8.02352941176471"/>
+    <col collapsed="false" hidden="false" max="257" min="9" style="27" width="14.2274509803922"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1" s="26">
@@ -45676,18 +45676,18 @@
   <dimension ref="A1:W6"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="A5:IV5 A1"/>
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="30" width="13.7019607843137"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="30" width="21.6901960784314"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="30" width="23.4352941176471"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="30" width="18.4039215686275"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="30" width="18.2235294117647"/>
-    <col collapsed="false" hidden="false" max="8" min="6" style="30" width="14.1529411764706"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="30" width="34.0078431372549"/>
-    <col collapsed="false" hidden="false" max="257" min="11" style="30" width="14.1529411764706"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="30" width="13.7764705882353"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="30" width="21.7960784313725"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="30" width="23.5529411764706"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="30" width="18.4941176470588"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="30" width="18.3137254901961"/>
+    <col collapsed="false" hidden="false" max="8" min="6" style="30" width="14.2274509803922"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="30" width="34.1803921568627"/>
+    <col collapsed="false" hidden="false" max="257" min="11" style="30" width="14.2274509803922"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="1" s="31">
@@ -45836,17 +45836,17 @@
   <dimension ref="A2:M4"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="H4" activeCellId="1" pane="topLeft" sqref="A5:IV5 H4"/>
+      <selection activeCell="H4" activeCellId="0" pane="topLeft" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="9.56862745098039"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="12.4823529411765"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="5" width="13.7294117647059"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="23.4352941176471"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="5" width="23.9764705882353"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="12.1372549019608"/>
-    <col collapsed="false" hidden="false" max="257" min="8" style="5" width="13.7294117647059"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="9.6156862745098"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="12.5450980392157"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="5" width="13.8"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="23.5529411764706"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="5" width="24.0941176470588"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="12.2"/>
+    <col collapsed="false" hidden="false" max="257" min="8" style="5" width="13.8"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="2" s="2"/>
@@ -45957,19 +45957,19 @@
   <dimension ref="A1:W6"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="A5:IV5 A1"/>
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="30" width="26.0313725490196"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="30" width="21.6901960784314"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="30" width="23.4352941176471"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="30" width="18.4039215686275"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="30" width="18.2235294117647"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="30" width="30.0352941176471"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="30" width="14.1529411764706"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="30" width="34.0078431372549"/>
-    <col collapsed="false" hidden="false" max="257" min="11" style="30" width="14.1529411764706"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="30" width="26.156862745098"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="30" width="21.7960784313725"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="30" width="23.5529411764706"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="30" width="18.4941176470588"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="30" width="18.3137254901961"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="30" width="30.1882352941176"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="30" width="14.2274509803922"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="30" width="34.1803921568627"/>
+    <col collapsed="false" hidden="false" max="257" min="11" style="30" width="14.2274509803922"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14" outlineLevel="0" r="1" s="31">
@@ -46115,13 +46115,13 @@
   <dimension ref="A1:V7"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="A5:IV5 A1"/>
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="23.3176470588235"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="42.0196078431373"/>
-    <col collapsed="false" hidden="false" max="257" min="3" style="7" width="14.1529411764706"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="23.4352941176471"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="42.2274509803922"/>
+    <col collapsed="false" hidden="false" max="257" min="3" style="7" width="14.2274509803922"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1" s="10">
@@ -46217,15 +46217,15 @@
   <dimension ref="A1:V23"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="A5:IV5 A1"/>
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="47.2313725490196"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="28.9764705882353"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="7" width="14.1529411764706"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="7" width="18.4039215686275"/>
-    <col collapsed="false" hidden="false" max="257" min="6" style="7" width="14.1529411764706"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="47.4627450980392"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="29.121568627451"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="7" width="14.2274509803922"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="7" width="18.4941176470588"/>
+    <col collapsed="false" hidden="false" max="257" min="6" style="7" width="14.2274509803922"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1" s="10">
@@ -46622,20 +46622,20 @@
   <dimension ref="A1:V43"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="G3" activeCellId="1" pane="topLeft" sqref="A5:IV5 G3"/>
+      <selection activeCell="G3" activeCellId="0" pane="topLeft" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="27" width="23.1529411764706"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="27" width="23.4352941176471"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="27" width="29.321568627451"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="27" width="11.7764705882353"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="27" width="8.14117647058824"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="27" width="25.3686274509804"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="27" width="16.6862745098039"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="25.3686274509804"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="16.6862745098039"/>
-    <col collapsed="false" hidden="false" max="257" min="12" style="27" width="14.1529411764706"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="27" width="23.2705882352941"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="27" width="23.5529411764706"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="27" width="29.4666666666667"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="27" width="11.8313725490196"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="27" width="8.1843137254902"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="27" width="25.4941176470588"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="27" width="16.7686274509804"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="25.4941176470588"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="16.7686274509804"/>
+    <col collapsed="false" hidden="false" max="257" min="12" style="27" width="14.2274509803922"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1" s="26">
@@ -47124,13 +47124,13 @@
   <dimension ref="A1:V11"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C5" activeCellId="0" pane="topLeft" sqref="A5:IV5"/>
+      <selection activeCell="C6" activeCellId="0" pane="topLeft" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="23.3176470588235"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="15.4549019607843"/>
-    <col collapsed="false" hidden="false" max="257" min="3" style="7" width="14.1529411764706"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="23.4352941176471"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="15.5294117647059"/>
+    <col collapsed="false" hidden="false" max="257" min="3" style="7" width="14.2274509803922"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1" s="10">
@@ -47199,7 +47199,9 @@
       <c r="B5" s="27" t="s">
         <v>1218</v>
       </c>
-      <c r="C5" s="27"/>
+      <c r="C5" s="27" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="6">
       <c r="A6" s="27" t="s">
@@ -47286,18 +47288,18 @@
   <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="F33" activeCellId="1" pane="topLeft" sqref="A5:IV5 F33"/>
+      <selection activeCell="F33" activeCellId="0" pane="topLeft" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="13.5294117647059"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="14.2274509803922"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="20.8823529411765"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="7" width="16.5254901960784"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="7" width="16.1607843137255"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="7" width="36.2392156862745"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="7" width="22.7294117647059"/>
-    <col collapsed="false" hidden="false" max="257" min="8" style="7" width="14.1529411764706"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="13.5921568627451"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="14.2980392156863"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="20.9843137254902"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="7" width="16.6039215686275"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="7" width="16.243137254902"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="7" width="36.4196078431373"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="7" width="22.8470588235294"/>
+    <col collapsed="false" hidden="false" max="257" min="8" style="7" width="14.2274509803922"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1" s="9">
@@ -48267,22 +48269,22 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="J5" activeCellId="0" pane="topLeft" sqref="A5:IV5"/>
+      <selection activeCell="J5" activeCellId="0" pane="topLeft" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="17.2666666666667"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="13.8470588235294"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="12.5725490196078"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="7" width="27.1254901960784"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="7" width="20.2666666666667"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="7" width="17.0666666666667"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="7" width="19.7607843137255"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="7" width="17.2666666666667"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="7" width="21.9960784313725"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="7" width="16.6509803921569"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="7" width="50.6117647058824"/>
-    <col collapsed="false" hidden="false" max="257" min="12" style="7" width="14.1529411764706"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="17.3450980392157"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="13.9176470588235"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="12.6352941176471"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="7" width="27.2588235294118"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="7" width="20.3686274509804"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="7" width="17.1490196078431"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="7" width="19.8627450980392"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="7" width="17.3450980392157"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="7" width="22.1058823529412"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="7" width="16.7333333333333"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="7" width="50.8666666666667"/>
+    <col collapsed="false" hidden="false" max="257" min="12" style="7" width="14.2274509803922"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1" s="10">
@@ -48624,14 +48626,14 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="F16" activeCellId="1" pane="topLeft" sqref="A5:IV5 F16"/>
+      <selection activeCell="F16" activeCellId="0" pane="topLeft" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="21.6901960784314"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="39.4313725490196"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="29.2666666666667"/>
-    <col collapsed="false" hidden="false" max="257" min="4" style="7" width="14.1529411764706"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="7" width="21.7960784313725"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="39.6313725490196"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="29.4117647058823"/>
+    <col collapsed="false" hidden="false" max="257" min="4" style="7" width="14.2274509803922"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1" s="8">
@@ -48716,17 +48718,17 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="A5:IV5 A1"/>
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="11" width="17.7725490196078"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="12" width="23.9764705882353"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="12" width="16.1607843137255"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="12" width="26.7176470588235"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="12" width="16.3254901960784"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="12" width="17.5294117647059"/>
-    <col collapsed="false" hidden="false" max="257" min="7" style="12" width="14.1529411764706"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="11" width="17.8627450980392"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="12" width="24.0941176470588"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="12" width="16.243137254902"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="12" width="26.8509803921569"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="12" width="16.4078431372549"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="12" width="17.6196078431373"/>
+    <col collapsed="false" hidden="false" max="257" min="7" style="12" width="14.2274509803922"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="11.6" outlineLevel="0" r="1" s="15">
@@ -48987,27 +48989,27 @@
   <dimension ref="A1:P21"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C11" activeCellId="1" pane="topLeft" sqref="A5:IV5 C11"/>
+      <selection activeCell="C11" activeCellId="0" pane="topLeft" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="12" width="23.9764705882353"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="12" width="14.1529411764706"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="12" width="11.4313725490196"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="12" width="18.4039215686275"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="12" width="23.3176470588235"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="12" width="20.1254901960784"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="12" width="15.6117647058824"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="12" width="16.1607843137255"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="12" width="15.8078431372549"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="12" width="16.6862745098039"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="12" width="13.2039215686275"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="12" width="20.1254901960784"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="12" width="30.2078431372549"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="12" width="14.2274509803922"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="12" width="14.1529411764706"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="16" width="19.9607843137255"/>
-    <col collapsed="false" hidden="false" max="257" min="17" style="12" width="14.1529411764706"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="12" width="24.0941176470588"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="12" width="14.2274509803922"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="12" width="11.4862745098039"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="12" width="18.4941176470588"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="12" width="23.4352941176471"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="12" width="20.2313725490196"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="12" width="15.6901960784314"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="12" width="16.243137254902"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="12" width="15.8823529411765"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="12" width="16.7686274509804"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="12" width="13.2666666666667"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="12" width="20.2313725490196"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="12" width="30.3607843137255"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="12" width="14.2980392156863"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="12" width="14.2274509803922"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="16" width="20.0588235294118"/>
+    <col collapsed="false" hidden="false" max="257" min="17" style="12" width="14.2274509803922"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="11.6" outlineLevel="0" r="1" s="15">
@@ -50069,19 +50071,19 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="D1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="G26" activeCellId="1" pane="topLeft" sqref="A5:IV5 G26"/>
+      <selection activeCell="G26" activeCellId="0" pane="topLeft" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="17" width="29.321568627451"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="17" width="42.2"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="17" width="47.3843137254902"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="17" width="19.6274509803922"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="17" width="33.5019607843137"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="17" width="14.1529411764706"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="17" width="26.4"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="17" width="24.0313725490196"/>
-    <col collapsed="false" hidden="false" max="257" min="9" style="17" width="14.1529411764706"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="17" width="29.4666666666667"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="17" width="42.4078431372549"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="17" width="47.6196078431373"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="17" width="19.7254901960784"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="17" width="33.6627450980392"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="17" width="14.2274509803922"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="17" width="26.5254901960784"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="17" width="24.1490196078431"/>
+    <col collapsed="false" hidden="false" max="257" min="9" style="17" width="14.2274509803922"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.8" outlineLevel="0" r="1" s="19">
@@ -50715,20 +50717,20 @@
   <dimension ref="A1:T14"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="A5:IV5 A1"/>
+      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="21" width="19.2745098039216"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="28.6"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="7.33333333333333"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="7" width="8.45490196078431"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="7" width="10.7529411764706"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="7" width="13.8"/>
-    <col collapsed="false" hidden="false" max="10" min="7" style="7" width="6.25098039215686"/>
-    <col collapsed="false" hidden="false" max="14" min="11" style="7" width="7.33333333333333"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="7" width="13.0156862745098"/>
-    <col collapsed="false" hidden="false" max="257" min="16" style="7" width="14.1529411764706"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="21" width="19.3725490196078"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="7" width="28.7411764705882"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="7" width="7.37254901960784"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="7" width="8.49411764705882"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="7" width="10.8078431372549"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="7" width="13.8745098039216"/>
+    <col collapsed="false" hidden="false" max="10" min="7" style="7" width="6.27843137254902"/>
+    <col collapsed="false" hidden="false" max="14" min="11" style="7" width="7.37254901960784"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="7" width="13.078431372549"/>
+    <col collapsed="false" hidden="false" max="257" min="16" style="7" width="14.2274509803922"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="true" customHeight="true" hidden="false" ht="13.05" outlineLevel="0" r="1" s="8">

</xml_diff>